<commit_message>
Add 1K resistor for CPU module USB 5V power
</commit_message>
<xml_diff>
--- a/PCB_files/IC905_USB_Band_Decoder_PCB_V1.0/IC905_Band_Decoder_BOM-20-Jan-2025.xlsx
+++ b/PCB_files/IC905_USB_Band_Decoder_PCB_V1.0/IC905_Band_Decoder_BOM-20-Jan-2025.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5578E9D6-5077-48CE-9232-2E67F6738419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD28D1AE-BADF-440B-8100-3CA7D1C2780E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="1095" windowWidth="21600" windowHeight="13275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="1650" windowWidth="26280" windowHeight="13275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_905_Band_Decoder_Band_Decod" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="183">
   <si>
     <t>No.</t>
   </si>
@@ -546,6 +546,24 @@
   </si>
   <si>
     <t>DIY</t>
+  </si>
+  <si>
+    <t>On CPU Module</t>
+  </si>
+  <si>
+    <t>1Kohm  0805 size resistor</t>
+  </si>
+  <si>
+    <t>various</t>
+  </si>
+  <si>
+    <t>PCB Version · K7MDL2/IC-905_Band_Decoder_on_ESP32-S3 Wiki</t>
+  </si>
+  <si>
+    <t>See Wiki</t>
+  </si>
+  <si>
+    <t>Value or size not critical</t>
   </si>
 </sst>
 </file>
@@ -959,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,6 +1812,35 @@
       </c>
       <c r="I30" s="3" t="s">
         <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D31" t="s">
+        <v>177</v>
+      </c>
+      <c r="E31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" t="s">
+        <v>182</v>
+      </c>
+      <c r="G31" t="s">
+        <v>179</v>
+      </c>
+      <c r="H31" t="s">
+        <v>181</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1822,9 +1869,10 @@
     <hyperlink ref="I2" r:id="rId22" xr:uid="{45E1E599-08F2-49D9-8EFA-B2EA383C4EC2}"/>
     <hyperlink ref="I27" r:id="rId23" xr:uid="{1BBE951E-833C-4EBC-8C28-762BA476C638}"/>
     <hyperlink ref="I30" r:id="rId24" xr:uid="{7289FDA1-35DC-4069-9EBF-216859C3C9E7}"/>
+    <hyperlink ref="I31" r:id="rId25" display="https://na01.safelinks.protection.outlook.com/?url=https%3A%2F%2Fgithub.com%2FK7MDL2%2FIC-905_Band_Decoder_on_ESP32-S3%2Fwiki%2FPCB-Version%231k-resistor-mod-to-cpu-board-for-5v-host-port-power&amp;data=05%7C02%7C%7C974029d92b6a4930565508dd545f4917%7C84df9e7fe9f640afb435aaaaaaaaaaaa%7C1%7C0%7C638759490414121356%7CUnknown%7CTWFpbGZsb3d8eyJFbXB0eU1hcGkiOnRydWUsIlYiOiIwLjAuMDAwMCIsIlAiOiJXaW4zMiIsIkFOIjoiTWFpbCIsIldUIjoyfQ%3D%3D%7C0%7C%7C%7C&amp;sdata=u0QpJT3Hjfa6uJPdZaf5cgTGxplQUPp3tzLPGiai1Xc%3D&amp;reserved=0" xr:uid="{1FCFE5F0-BA2F-4ECB-AE18-BBB3C488AB86}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>